<commit_message>
basic Ficks code done and running
</commit_message>
<xml_diff>
--- a/step_by_step_model.xlsx
+++ b/step_by_step_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/Library/CloudStorage/iCloud Drive/Documents/Summer/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1FF734-A7AE-214B-9D46-31585F4559A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD62A5C9-78AE-E94F-B35A-408702665329}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1180" windowWidth="25440" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="1180" windowWidth="25440" windowHeight="16780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>son of sevenless protein</t>
   </si>
   <si>
-    <t>Sos =&gt; Ras</t>
-  </si>
-  <si>
     <t>Ras</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>FPR1 =&gt; Sos</t>
+  </si>
+  <si>
+    <t>Sos ===&gt; Ras</t>
   </si>
 </sst>
 </file>
@@ -715,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DK33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -993,10 +993,10 @@
         <v>41</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>46</v>
       </c>
       <c r="D7" s="19">
         <v>0</v>
@@ -1736,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AY123"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2034,7 +2034,7 @@
         <v>38</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="15">
         <v>1</v>
@@ -2099,7 +2099,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D7" s="15">
         <v>1</v>

</xml_diff>